<commit_message>
Issue #11080 - Cal Sheet Corrections - Non-numerical values in OPTAA cal arrays
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GI01SUMO_00003.xlsx
+++ b/deployment/Omaha_Cal_Info_GI01SUMO_00003.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="611">
   <si>
     <t>Mooring OOIBARCODE</t>
   </si>
@@ -1761,476 +1761,255 @@
     <t>GI01SUMO-00003-DCL16</t>
   </si>
   <si>
-    <t>0.03813300]</t>
+    <t>0.00221700</t>
   </si>
   <si>
-    <t>0.02979400]</t>
+    <t>0.00550500</t>
   </si>
   <si>
-    <t>0.01998400]</t>
+    <t>0.00773700</t>
   </si>
   <si>
-    <t>0.01485500]</t>
+    <t>0.00617600</t>
   </si>
   <si>
-    <t>0.00943800]</t>
+    <t>0.00474300</t>
   </si>
   <si>
-    <t>0.00523000]</t>
+    <t>0.00483600</t>
   </si>
   <si>
-    <t>0.00372900]</t>
+    <t>0.00796300</t>
   </si>
   <si>
-    <t>0.00384400]</t>
+    <t>0.00375800</t>
   </si>
   <si>
-    <t>0.00279300]</t>
+    <t>0.00670500</t>
   </si>
   <si>
-    <t>0.00232100]</t>
+    <t>0.00559300</t>
   </si>
   <si>
-    <t>0.00168000]</t>
+    <t>0.00444700</t>
   </si>
   <si>
-    <t>0.00177100]</t>
+    <t>0.00501700</t>
   </si>
   <si>
-    <t>0.00239500]</t>
+    <t>0.00410900</t>
   </si>
   <si>
-    <t>0.00166600]</t>
+    <t>0.00384400</t>
   </si>
   <si>
-    <t>0.00138900]</t>
+    <t>0.00476800</t>
   </si>
   <si>
-    <t>0.00185500]</t>
+    <t>0.00431900</t>
   </si>
   <si>
-    <t>0.00115700]</t>
+    <t>0.00398800</t>
   </si>
   <si>
-    <t>0.00114800]</t>
+    <t>0.00401900</t>
   </si>
   <si>
-    <t>0.00127500]</t>
+    <t>0.00346600</t>
   </si>
   <si>
-    <t>0.00107900]</t>
+    <t>0.00370600</t>
   </si>
   <si>
-    <t>0.00114500]</t>
+    <t>0.00367200</t>
   </si>
   <si>
-    <t>0.00087300]</t>
+    <t>0.00315500</t>
   </si>
   <si>
-    <t>0.00089700]</t>
+    <t>0.00396300</t>
   </si>
   <si>
-    <t>0.00065700]</t>
+    <t>0.00357500</t>
   </si>
   <si>
-    <t>0.00068900]</t>
+    <t>0.00317300</t>
   </si>
   <si>
-    <t>0.00066800]</t>
+    <t>0.00324100</t>
   </si>
   <si>
-    <t>0.00062100]</t>
+    <t>0.00339000</t>
   </si>
   <si>
-    <t>0.00053800]</t>
+    <t>0.00248900</t>
   </si>
   <si>
-    <t>0.00042400]</t>
+    <t>0.00327800</t>
   </si>
   <si>
-    <t>0.00067300]</t>
+    <t>0.00296700</t>
   </si>
   <si>
-    <t>0.00050100]</t>
+    <t>0.00305700</t>
   </si>
   <si>
-    <t>0.00037000]</t>
+    <t>0.00275100</t>
   </si>
   <si>
-    <t>0.00032100]</t>
+    <t>0.00277900</t>
   </si>
   <si>
-    <t>0.00036900]</t>
+    <t>0.00268100</t>
   </si>
   <si>
-    <t>0.00035600]</t>
+    <t>0.00245500</t>
   </si>
   <si>
-    <t>0.00032800]</t>
+    <t>0.00280000</t>
   </si>
   <si>
-    <t>0.00019700]</t>
+    <t>0.00238300</t>
   </si>
   <si>
-    <t>0.00030000]</t>
+    <t>0.00228300</t>
   </si>
   <si>
-    <t>0.00044900]</t>
+    <t>0.00252700</t>
   </si>
   <si>
-    <t>0.00027000]</t>
+    <t>0.00201500</t>
   </si>
   <si>
-    <t>0.00033900]</t>
+    <t>0.00227000</t>
   </si>
   <si>
-    <t>0.00055400]</t>
+    <t>0.00214800</t>
   </si>
   <si>
-    <t>0.00061300]</t>
+    <t>0.00182100</t>
   </si>
   <si>
-    <t>0.00048300]</t>
+    <t>0.00197000</t>
   </si>
   <si>
-    <t>0.00062600]</t>
+    <t>0.00171500</t>
   </si>
   <si>
-    <t>0.00015300]</t>
+    <t>0.00177100</t>
   </si>
   <si>
-    <t>0.00023700]</t>
+    <t>0.00178600</t>
   </si>
   <si>
-    <t>0.00024100]</t>
+    <t>0.00158200</t>
   </si>
   <si>
-    <t>0.00038500]</t>
+    <t>0.00169300</t>
   </si>
   <si>
-    <t>0.00029400]</t>
+    <t>0.00145400</t>
   </si>
   <si>
-    <t>0.00027400]</t>
+    <t>0.00144900</t>
   </si>
   <si>
-    <t>0.00023500]</t>
+    <t>0.00147400</t>
   </si>
   <si>
-    <t>0.00018600]</t>
+    <t>0.00148700</t>
   </si>
   <si>
-    <t>0.00013000]</t>
+    <t>0.00149000</t>
   </si>
   <si>
-    <t>0.00033300]</t>
+    <t>0.00128600</t>
   </si>
   <si>
-    <t>0.00029900]</t>
+    <t>0.00148800</t>
   </si>
   <si>
-    <t>0.00018500]</t>
+    <t>0.00129200</t>
   </si>
   <si>
-    <t>0.00007600]</t>
+    <t>0.00133500</t>
   </si>
   <si>
-    <t>0.00021400]</t>
+    <t>0.00137900</t>
   </si>
   <si>
-    <t>0.00010900]</t>
+    <t>0.00113400</t>
   </si>
   <si>
-    <t>0.00005300]</t>
+    <t>0.00152300</t>
   </si>
   <si>
-    <t>0.00008000]</t>
+    <t>0.00136900</t>
   </si>
   <si>
-    <t>-0.00001700]</t>
+    <t>0.00116400</t>
   </si>
   <si>
-    <t>0.00007000]</t>
+    <t>0.00151700</t>
   </si>
   <si>
-    <t>0.00014900]</t>
+    <t>0.00114300</t>
   </si>
   <si>
-    <t>-0.00002200]</t>
+    <t>0.00085800</t>
   </si>
   <si>
-    <t>0.00002000]</t>
+    <t>0.00128300</t>
   </si>
   <si>
-    <t>0.00003900]</t>
+    <t>0.00071900</t>
   </si>
   <si>
-    <t>0.00001700]</t>
+    <t>0.00098700</t>
   </si>
   <si>
-    <t>0.00016100]</t>
+    <t>0.00081000</t>
   </si>
   <si>
-    <t>0.00001400]</t>
+    <t>0.00033000</t>
   </si>
   <si>
-    <t>0.00041000]</t>
+    <t>0.00078100</t>
   </si>
   <si>
-    <t>0.00043100]</t>
+    <t>0.00034200</t>
   </si>
   <si>
-    <t>0.00058000]</t>
+    <t>0.00031200</t>
   </si>
   <si>
-    <t>0.00043700]</t>
+    <t>0.00039600</t>
   </si>
   <si>
-    <t>0.00018500]]</t>
+    <t>0.00045500</t>
   </si>
   <si>
-    <t>0.00221700]</t>
+    <t>-0.00002600</t>
   </si>
   <si>
-    <t>0.00550500]</t>
+    <t>0.00054000</t>
   </si>
   <si>
-    <t>0.00773700]</t>
-  </si>
-  <si>
-    <t>0.00617600]</t>
-  </si>
-  <si>
-    <t>0.00474300]</t>
-  </si>
-  <si>
-    <t>0.00483600]</t>
-  </si>
-  <si>
-    <t>0.00796300]</t>
-  </si>
-  <si>
-    <t>0.00375800]</t>
-  </si>
-  <si>
-    <t>0.00670500]</t>
-  </si>
-  <si>
-    <t>0.00559300]</t>
-  </si>
-  <si>
-    <t>0.00444700]</t>
-  </si>
-  <si>
-    <t>0.00501700]</t>
-  </si>
-  <si>
-    <t>0.00410900]</t>
-  </si>
-  <si>
-    <t>0.00476800]</t>
-  </si>
-  <si>
-    <t>0.00431900]</t>
-  </si>
-  <si>
-    <t>0.00398800]</t>
-  </si>
-  <si>
-    <t>0.00401900]</t>
-  </si>
-  <si>
-    <t>0.00346600]</t>
-  </si>
-  <si>
-    <t>0.00370600]</t>
-  </si>
-  <si>
-    <t>0.00367200]</t>
-  </si>
-  <si>
-    <t>0.00315500]</t>
-  </si>
-  <si>
-    <t>0.00396300]</t>
-  </si>
-  <si>
-    <t>0.00357500]</t>
-  </si>
-  <si>
-    <t>0.00317300]</t>
-  </si>
-  <si>
-    <t>0.00324100]</t>
-  </si>
-  <si>
-    <t>0.00339000]</t>
-  </si>
-  <si>
-    <t>0.00248900]</t>
-  </si>
-  <si>
-    <t>0.00327800]</t>
-  </si>
-  <si>
-    <t>0.00296700]</t>
-  </si>
-  <si>
-    <t>0.00305700]</t>
-  </si>
-  <si>
-    <t>0.00275100]</t>
-  </si>
-  <si>
-    <t>0.00277900]</t>
-  </si>
-  <si>
-    <t>0.00268100]</t>
-  </si>
-  <si>
-    <t>0.00245500]</t>
-  </si>
-  <si>
-    <t>0.00280000]</t>
-  </si>
-  <si>
-    <t>0.00238300]</t>
-  </si>
-  <si>
-    <t>0.00228300]</t>
-  </si>
-  <si>
-    <t>0.00252700]</t>
-  </si>
-  <si>
-    <t>0.00201500]</t>
-  </si>
-  <si>
-    <t>0.00227000]</t>
-  </si>
-  <si>
-    <t>0.00214800]</t>
-  </si>
-  <si>
-    <t>0.00182100]</t>
-  </si>
-  <si>
-    <t>0.00197000]</t>
-  </si>
-  <si>
-    <t>0.00171500]</t>
-  </si>
-  <si>
-    <t>0.00178600]</t>
-  </si>
-  <si>
-    <t>0.00158200]</t>
-  </si>
-  <si>
-    <t>0.00169300]</t>
-  </si>
-  <si>
-    <t>0.00145400]</t>
-  </si>
-  <si>
-    <t>0.00144900]</t>
-  </si>
-  <si>
-    <t>0.00147400]</t>
-  </si>
-  <si>
-    <t>0.00148700]</t>
-  </si>
-  <si>
-    <t>0.00149000]</t>
-  </si>
-  <si>
-    <t>0.00128600]</t>
-  </si>
-  <si>
-    <t>0.00148800]</t>
-  </si>
-  <si>
-    <t>0.00129200]</t>
-  </si>
-  <si>
-    <t>0.00133500]</t>
-  </si>
-  <si>
-    <t>0.00137900]</t>
-  </si>
-  <si>
-    <t>0.00113400]</t>
-  </si>
-  <si>
-    <t>0.00152300]</t>
-  </si>
-  <si>
-    <t>0.00136900]</t>
-  </si>
-  <si>
-    <t>0.00116400]</t>
-  </si>
-  <si>
-    <t>0.00151700]</t>
-  </si>
-  <si>
-    <t>0.00114300]</t>
-  </si>
-  <si>
-    <t>0.00085800]</t>
-  </si>
-  <si>
-    <t>0.00128300]</t>
-  </si>
-  <si>
-    <t>0.00071900]</t>
-  </si>
-  <si>
-    <t>0.00098700]</t>
-  </si>
-  <si>
-    <t>0.00081000]</t>
-  </si>
-  <si>
-    <t>0.00033000]</t>
-  </si>
-  <si>
-    <t>0.00078100]</t>
-  </si>
-  <si>
-    <t>0.00034200]</t>
-  </si>
-  <si>
-    <t>0.00031200]</t>
-  </si>
-  <si>
-    <t>0.00039600]</t>
-  </si>
-  <si>
-    <t>0.00045500]</t>
-  </si>
-  <si>
-    <t>-0.00002600]</t>
-  </si>
-  <si>
-    <t>0.00054000]</t>
-  </si>
-  <si>
-    <t>-0.00082800]]</t>
+    <t>-0.00082800</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="d&quot;-&quot;mmm&quot;-&quot;yy"/>
     <numFmt numFmtId="60" formatCode="h:mm:ss&quot; &quot;AM/PM"/>
     <numFmt numFmtId="61" formatCode="0.0000E+00"/>
     <numFmt numFmtId="62" formatCode="0.000"/>
     <numFmt numFmtId="63" formatCode="0.0000"/>
+    <numFmt numFmtId="64" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -2617,7 +2396,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -2633,10 +2412,10 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2669,7 +2448,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2684,10 +2463,10 @@
     <xf numFmtId="14" fontId="3" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -2744,7 +2523,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2777,7 +2556,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2807,7 +2586,7 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2843,7 +2622,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2864,13 +2643,13 @@
     <xf numFmtId="2" fontId="3" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="6" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2946,6 +2725,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -3127,9 +2909,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -3209,7 +2991,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -3237,10 +3019,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -3496,9 +3278,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -3786,7 +3568,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -3814,10 +3596,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -47527,7 +47309,7 @@
     <col min="33" max="33" width="9.67188" style="109" customWidth="1"/>
     <col min="34" max="34" width="9.67188" style="109" customWidth="1"/>
     <col min="35" max="35" width="9.67188" style="109" customWidth="1"/>
-    <col min="36" max="36" width="9.67188" style="109" customWidth="1"/>
+    <col min="36" max="36" width="11" style="109" customWidth="1"/>
     <col min="37" max="256" width="11.5" style="109" customWidth="1"/>
   </cols>
   <sheetData>
@@ -47637,8 +47419,8 @@
       <c r="AI1" s="104">
         <v>0.037302</v>
       </c>
-      <c r="AJ1" t="s" s="36">
-        <v>532</v>
+      <c r="AJ1" s="110">
+        <v>0.038133</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1">
@@ -47747,8 +47529,8 @@
       <c r="AI2" s="104">
         <v>0.02928</v>
       </c>
-      <c r="AJ2" t="s" s="36">
-        <v>533</v>
+      <c r="AJ2" s="110">
+        <v>0.029794</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
@@ -47857,8 +47639,8 @@
       <c r="AI3" s="104">
         <v>0.020236</v>
       </c>
-      <c r="AJ3" t="s" s="36">
-        <v>534</v>
+      <c r="AJ3" s="110">
+        <v>0.019984</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
@@ -47967,8 +47749,8 @@
       <c r="AI4" s="104">
         <v>0.013874</v>
       </c>
-      <c r="AJ4" t="s" s="36">
-        <v>535</v>
+      <c r="AJ4" s="110">
+        <v>0.014855</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
@@ -48077,8 +47859,8 @@
       <c r="AI5" s="104">
         <v>0.008467000000000001</v>
       </c>
-      <c r="AJ5" t="s" s="36">
-        <v>536</v>
+      <c r="AJ5" s="110">
+        <v>0.009438</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
@@ -48187,8 +47969,8 @@
       <c r="AI6" s="104">
         <v>0.006114</v>
       </c>
-      <c r="AJ6" t="s" s="36">
-        <v>537</v>
+      <c r="AJ6" s="110">
+        <v>0.00523</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
@@ -48297,8 +48079,8 @@
       <c r="AI7" s="104">
         <v>0.004266</v>
       </c>
-      <c r="AJ7" t="s" s="36">
-        <v>538</v>
+      <c r="AJ7" s="110">
+        <v>0.003729</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">
@@ -48407,8 +48189,8 @@
       <c r="AI8" s="104">
         <v>0.003296</v>
       </c>
-      <c r="AJ8" t="s" s="36">
-        <v>539</v>
+      <c r="AJ8" s="110">
+        <v>0.003844</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1">
@@ -48517,8 +48299,8 @@
       <c r="AI9" s="104">
         <v>0.002927</v>
       </c>
-      <c r="AJ9" t="s" s="36">
-        <v>540</v>
+      <c r="AJ9" s="110">
+        <v>0.002793</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
@@ -48627,8 +48409,8 @@
       <c r="AI10" s="104">
         <v>0.002433</v>
       </c>
-      <c r="AJ10" t="s" s="36">
-        <v>541</v>
+      <c r="AJ10" s="110">
+        <v>0.002321</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1">
@@ -48737,8 +48519,8 @@
       <c r="AI11" s="104">
         <v>0.002677</v>
       </c>
-      <c r="AJ11" t="s" s="36">
-        <v>542</v>
+      <c r="AJ11" s="110">
+        <v>0.00168</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1">
@@ -48847,8 +48629,8 @@
       <c r="AI12" s="104">
         <v>0.002057</v>
       </c>
-      <c r="AJ12" t="s" s="36">
-        <v>543</v>
+      <c r="AJ12" s="110">
+        <v>0.001771</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1">
@@ -48957,8 +48739,8 @@
       <c r="AI13" s="104">
         <v>0.00191</v>
       </c>
-      <c r="AJ13" t="s" s="36">
-        <v>544</v>
+      <c r="AJ13" s="110">
+        <v>0.002395</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1">
@@ -49067,8 +48849,8 @@
       <c r="AI14" s="104">
         <v>0.001863</v>
       </c>
-      <c r="AJ14" t="s" s="36">
-        <v>545</v>
+      <c r="AJ14" s="110">
+        <v>0.001666</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1">
@@ -49177,8 +48959,8 @@
       <c r="AI15" s="104">
         <v>0.001539</v>
       </c>
-      <c r="AJ15" t="s" s="36">
-        <v>546</v>
+      <c r="AJ15" s="110">
+        <v>0.001389</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1">
@@ -49287,8 +49069,8 @@
       <c r="AI16" s="104">
         <v>0.001363</v>
       </c>
-      <c r="AJ16" t="s" s="36">
-        <v>547</v>
+      <c r="AJ16" s="110">
+        <v>0.001855</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1">
@@ -49397,8 +49179,8 @@
       <c r="AI17" s="104">
         <v>0.001349</v>
       </c>
-      <c r="AJ17" t="s" s="36">
-        <v>548</v>
+      <c r="AJ17" s="110">
+        <v>0.001157</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1">
@@ -49507,8 +49289,8 @@
       <c r="AI18" s="104">
         <v>0.001274</v>
       </c>
-      <c r="AJ18" t="s" s="36">
-        <v>549</v>
+      <c r="AJ18" s="110">
+        <v>0.001148</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1">
@@ -49617,8 +49399,8 @@
       <c r="AI19" s="104">
         <v>0.001317</v>
       </c>
-      <c r="AJ19" t="s" s="36">
-        <v>550</v>
+      <c r="AJ19" s="110">
+        <v>0.001275</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1">
@@ -49727,8 +49509,8 @@
       <c r="AI20" s="104">
         <v>0.001091</v>
       </c>
-      <c r="AJ20" t="s" s="36">
-        <v>551</v>
+      <c r="AJ20" s="110">
+        <v>0.001079</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1">
@@ -49837,8 +49619,8 @@
       <c r="AI21" s="104">
         <v>0.001011</v>
       </c>
-      <c r="AJ21" t="s" s="36">
-        <v>552</v>
+      <c r="AJ21" s="110">
+        <v>0.001145</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1">
@@ -49947,8 +49729,8 @@
       <c r="AI22" s="104">
         <v>0.000973</v>
       </c>
-      <c r="AJ22" t="s" s="36">
-        <v>553</v>
+      <c r="AJ22" s="110">
+        <v>0.000873</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1">
@@ -50057,8 +49839,8 @@
       <c r="AI23" s="104">
         <v>0.000918</v>
       </c>
-      <c r="AJ23" t="s" s="36">
-        <v>554</v>
+      <c r="AJ23" s="110">
+        <v>0.000897</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1">
@@ -50167,8 +49949,8 @@
       <c r="AI24" s="104">
         <v>0.000861</v>
       </c>
-      <c r="AJ24" t="s" s="36">
-        <v>555</v>
+      <c r="AJ24" s="110">
+        <v>0.000657</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1">
@@ -50277,8 +50059,8 @@
       <c r="AI25" s="104">
         <v>0.0008720000000000001</v>
       </c>
-      <c r="AJ25" t="s" s="36">
-        <v>556</v>
+      <c r="AJ25" s="110">
+        <v>0.0006890000000000001</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1">
@@ -50387,8 +50169,8 @@
       <c r="AI26" s="104">
         <v>0.000729</v>
       </c>
-      <c r="AJ26" t="s" s="36">
-        <v>557</v>
+      <c r="AJ26" s="110">
+        <v>0.000668</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1">
@@ -50497,8 +50279,8 @@
       <c r="AI27" s="104">
         <v>0.000632</v>
       </c>
-      <c r="AJ27" t="s" s="36">
-        <v>558</v>
+      <c r="AJ27" s="110">
+        <v>0.000621</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1">
@@ -50607,8 +50389,8 @@
       <c r="AI28" s="104">
         <v>0.000627</v>
       </c>
-      <c r="AJ28" t="s" s="36">
-        <v>559</v>
+      <c r="AJ28" s="110">
+        <v>0.000538</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1">
@@ -50717,8 +50499,8 @@
       <c r="AI29" s="104">
         <v>0.00051</v>
       </c>
-      <c r="AJ29" t="s" s="36">
-        <v>560</v>
+      <c r="AJ29" s="110">
+        <v>0.000424</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1">
@@ -50827,8 +50609,8 @@
       <c r="AI30" s="104">
         <v>0.000499</v>
       </c>
-      <c r="AJ30" t="s" s="36">
-        <v>561</v>
+      <c r="AJ30" s="110">
+        <v>0.000673</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1">
@@ -50937,8 +50719,8 @@
       <c r="AI31" s="104">
         <v>0.000468</v>
       </c>
-      <c r="AJ31" t="s" s="36">
-        <v>562</v>
+      <c r="AJ31" s="110">
+        <v>0.000501</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1">
@@ -51047,8 +50829,8 @@
       <c r="AI32" s="104">
         <v>0.000389</v>
       </c>
-      <c r="AJ32" t="s" s="36">
-        <v>563</v>
+      <c r="AJ32" s="110">
+        <v>0.00037</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1">
@@ -51157,8 +50939,8 @@
       <c r="AI33" s="104">
         <v>0.000384</v>
       </c>
-      <c r="AJ33" t="s" s="36">
-        <v>564</v>
+      <c r="AJ33" s="110">
+        <v>0.000321</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1">
@@ -51267,8 +51049,8 @@
       <c r="AI34" s="104">
         <v>0.000442</v>
       </c>
-      <c r="AJ34" t="s" s="36">
-        <v>565</v>
+      <c r="AJ34" s="110">
+        <v>0.000369</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1">
@@ -51377,8 +51159,8 @@
       <c r="AI35" s="104">
         <v>0.000395</v>
       </c>
-      <c r="AJ35" t="s" s="36">
-        <v>566</v>
+      <c r="AJ35" s="110">
+        <v>0.000356</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1">
@@ -51487,8 +51269,8 @@
       <c r="AI36" s="104">
         <v>0.000354</v>
       </c>
-      <c r="AJ36" t="s" s="36">
-        <v>567</v>
+      <c r="AJ36" s="110">
+        <v>0.000328</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1">
@@ -51597,8 +51379,8 @@
       <c r="AI37" s="104">
         <v>0.000296</v>
       </c>
-      <c r="AJ37" t="s" s="36">
-        <v>568</v>
+      <c r="AJ37" s="110">
+        <v>0.000197</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1">
@@ -51707,8 +51489,8 @@
       <c r="AI38" s="104">
         <v>0.000353</v>
       </c>
-      <c r="AJ38" t="s" s="36">
-        <v>569</v>
+      <c r="AJ38" s="110">
+        <v>0.0003</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1">
@@ -51817,8 +51599,8 @@
       <c r="AI39" s="104">
         <v>0.000306</v>
       </c>
-      <c r="AJ39" t="s" s="36">
-        <v>570</v>
+      <c r="AJ39" s="110">
+        <v>0.000449</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1">
@@ -51927,8 +51709,8 @@
       <c r="AI40" s="104">
         <v>0.000383</v>
       </c>
-      <c r="AJ40" t="s" s="36">
-        <v>571</v>
+      <c r="AJ40" s="110">
+        <v>0.00027</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1">
@@ -52037,8 +51819,8 @@
       <c r="AI41" s="104">
         <v>0.000457</v>
       </c>
-      <c r="AJ41" t="s" s="36">
-        <v>568</v>
+      <c r="AJ41" s="110">
+        <v>0.000197</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1">
@@ -52147,8 +51929,8 @@
       <c r="AI42" s="104">
         <v>0.000497</v>
       </c>
-      <c r="AJ42" t="s" s="36">
-        <v>572</v>
+      <c r="AJ42" s="110">
+        <v>0.000339</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1">
@@ -52257,8 +52039,8 @@
       <c r="AI43" s="104">
         <v>0.000525</v>
       </c>
-      <c r="AJ43" t="s" s="36">
-        <v>573</v>
+      <c r="AJ43" s="110">
+        <v>0.000554</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1">
@@ -52367,8 +52149,8 @@
       <c r="AI44" s="104">
         <v>0.000578</v>
       </c>
-      <c r="AJ44" t="s" s="36">
-        <v>562</v>
+      <c r="AJ44" s="110">
+        <v>0.000501</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1">
@@ -52477,8 +52259,8 @@
       <c r="AI45" s="104">
         <v>0.000619</v>
       </c>
-      <c r="AJ45" t="s" s="36">
-        <v>574</v>
+      <c r="AJ45" s="110">
+        <v>0.000613</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1">
@@ -52587,8 +52369,8 @@
       <c r="AI46" s="104">
         <v>0.000605</v>
       </c>
-      <c r="AJ46" t="s" s="36">
-        <v>575</v>
+      <c r="AJ46" s="110">
+        <v>0.000483</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1">
@@ -52697,8 +52479,8 @@
       <c r="AI47" s="104">
         <v>0.000647</v>
       </c>
-      <c r="AJ47" t="s" s="36">
-        <v>576</v>
+      <c r="AJ47" s="110">
+        <v>0.000626</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1">
@@ -52807,8 +52589,8 @@
       <c r="AI48" s="104">
         <v>0.000285</v>
       </c>
-      <c r="AJ48" t="s" s="36">
-        <v>577</v>
+      <c r="AJ48" s="110">
+        <v>0.000153</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1">
@@ -52917,8 +52699,8 @@
       <c r="AI49" s="104">
         <v>0.000276</v>
       </c>
-      <c r="AJ49" t="s" s="36">
-        <v>578</v>
+      <c r="AJ49" s="110">
+        <v>0.000237</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1">
@@ -53027,8 +52809,8 @@
       <c r="AI50" s="104">
         <v>0.000293</v>
       </c>
-      <c r="AJ50" t="s" s="36">
-        <v>579</v>
+      <c r="AJ50" s="110">
+        <v>0.000241</v>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1">
@@ -53137,8 +52919,8 @@
       <c r="AI51" s="104">
         <v>0.000279</v>
       </c>
-      <c r="AJ51" t="s" s="36">
-        <v>580</v>
+      <c r="AJ51" s="110">
+        <v>0.000385</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1">
@@ -53247,8 +53029,8 @@
       <c r="AI52" s="104">
         <v>0.000248</v>
       </c>
-      <c r="AJ52" t="s" s="36">
-        <v>581</v>
+      <c r="AJ52" s="110">
+        <v>0.000294</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1">
@@ -53357,8 +53139,8 @@
       <c r="AI53" s="104">
         <v>0.000261</v>
       </c>
-      <c r="AJ53" t="s" s="36">
-        <v>582</v>
+      <c r="AJ53" s="110">
+        <v>0.000274</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1">
@@ -53467,8 +53249,8 @@
       <c r="AI54" s="104">
         <v>0.000202</v>
       </c>
-      <c r="AJ54" t="s" s="36">
-        <v>583</v>
+      <c r="AJ54" s="110">
+        <v>0.000235</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1">
@@ -53577,8 +53359,8 @@
       <c r="AI55" s="104">
         <v>0.000279</v>
       </c>
-      <c r="AJ55" t="s" s="36">
-        <v>584</v>
+      <c r="AJ55" s="110">
+        <v>0.000186</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1">
@@ -53687,8 +53469,8 @@
       <c r="AI56" s="104">
         <v>0.000208</v>
       </c>
-      <c r="AJ56" t="s" s="36">
-        <v>585</v>
+      <c r="AJ56" s="110">
+        <v>0.00013</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1">
@@ -53797,8 +53579,8 @@
       <c r="AI57" s="104">
         <v>0.000253</v>
       </c>
-      <c r="AJ57" t="s" s="36">
-        <v>586</v>
+      <c r="AJ57" s="110">
+        <v>0.000333</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1">
@@ -53907,8 +53689,8 @@
       <c r="AI58" s="104">
         <v>0.00027</v>
       </c>
-      <c r="AJ58" t="s" s="36">
-        <v>587</v>
+      <c r="AJ58" s="110">
+        <v>0.000299</v>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1">
@@ -54017,8 +53799,8 @@
       <c r="AI59" s="104">
         <v>0.000194</v>
       </c>
-      <c r="AJ59" t="s" s="36">
-        <v>588</v>
+      <c r="AJ59" s="110">
+        <v>0.000185</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1">
@@ -54127,8 +53909,8 @@
       <c r="AI60" s="104">
         <v>0.000187</v>
       </c>
-      <c r="AJ60" t="s" s="36">
-        <v>589</v>
+      <c r="AJ60" s="110">
+        <v>7.6e-05</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1">
@@ -54237,8 +54019,8 @@
       <c r="AI61" s="104">
         <v>0.000231</v>
       </c>
-      <c r="AJ61" t="s" s="36">
-        <v>590</v>
+      <c r="AJ61" s="110">
+        <v>0.000214</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1">
@@ -54347,8 +54129,8 @@
       <c r="AI62" s="104">
         <v>0.000212</v>
       </c>
-      <c r="AJ62" t="s" s="36">
-        <v>587</v>
+      <c r="AJ62" s="110">
+        <v>0.000299</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1">
@@ -54457,8 +54239,8 @@
       <c r="AI63" s="104">
         <v>0.000205</v>
       </c>
-      <c r="AJ63" t="s" s="36">
-        <v>591</v>
+      <c r="AJ63" s="110">
+        <v>0.000109</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1">
@@ -54567,8 +54349,8 @@
       <c r="AI64" s="104">
         <v>0.00015</v>
       </c>
-      <c r="AJ64" t="s" s="36">
-        <v>592</v>
+      <c r="AJ64" s="110">
+        <v>5.3e-05</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1">
@@ -54677,8 +54459,8 @@
       <c r="AI65" s="104">
         <v>0.00013</v>
       </c>
-      <c r="AJ65" t="s" s="36">
-        <v>593</v>
+      <c r="AJ65" s="110">
+        <v>8.000000000000001e-05</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1">
@@ -54787,8 +54569,8 @@
       <c r="AI66" s="104">
         <v>5.1e-05</v>
       </c>
-      <c r="AJ66" t="s" s="36">
-        <v>594</v>
+      <c r="AJ66" s="110">
+        <v>-1.7e-05</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1">
@@ -54897,8 +54679,8 @@
       <c r="AI67" s="104">
         <v>4.1e-05</v>
       </c>
-      <c r="AJ67" t="s" s="36">
-        <v>595</v>
+      <c r="AJ67" s="110">
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1">
@@ -55007,8 +54789,8 @@
       <c r="AI68" s="104">
         <v>-3e-06</v>
       </c>
-      <c r="AJ68" t="s" s="36">
-        <v>596</v>
+      <c r="AJ68" s="110">
+        <v>0.000149</v>
       </c>
     </row>
     <row r="69" ht="15" customHeight="1">
@@ -55117,8 +54899,8 @@
       <c r="AI69" s="104">
         <v>-9.1e-05</v>
       </c>
-      <c r="AJ69" t="s" s="36">
-        <v>597</v>
+      <c r="AJ69" s="110">
+        <v>-2.2e-05</v>
       </c>
     </row>
     <row r="70" ht="15" customHeight="1">
@@ -55227,8 +55009,8 @@
       <c r="AI70" s="104">
         <v>-1e-05</v>
       </c>
-      <c r="AJ70" t="s" s="36">
-        <v>598</v>
+      <c r="AJ70" s="110">
+        <v>2e-05</v>
       </c>
     </row>
     <row r="71" ht="15" customHeight="1">
@@ -55337,8 +55119,8 @@
       <c r="AI71" s="104">
         <v>3.3e-05</v>
       </c>
-      <c r="AJ71" t="s" s="36">
-        <v>599</v>
+      <c r="AJ71" s="110">
+        <v>3.9e-05</v>
       </c>
     </row>
     <row r="72" ht="15" customHeight="1">
@@ -55447,8 +55229,8 @@
       <c r="AI72" s="104">
         <v>9.500000000000001e-05</v>
       </c>
-      <c r="AJ72" t="s" s="36">
-        <v>600</v>
+      <c r="AJ72" s="110">
+        <v>1.7e-05</v>
       </c>
     </row>
     <row r="73" ht="15" customHeight="1">
@@ -55557,8 +55339,8 @@
       <c r="AI73" s="104">
         <v>0.00018</v>
       </c>
-      <c r="AJ73" t="s" s="36">
-        <v>601</v>
+      <c r="AJ73" s="110">
+        <v>0.000161</v>
       </c>
     </row>
     <row r="74" ht="15" customHeight="1">
@@ -55667,8 +55449,8 @@
       <c r="AI74" s="104">
         <v>0.000187</v>
       </c>
-      <c r="AJ74" t="s" s="36">
-        <v>602</v>
+      <c r="AJ74" s="110">
+        <v>1.4e-05</v>
       </c>
     </row>
     <row r="75" ht="15" customHeight="1">
@@ -55777,8 +55559,8 @@
       <c r="AI75" s="104">
         <v>0.000335</v>
       </c>
-      <c r="AJ75" t="s" s="36">
-        <v>603</v>
+      <c r="AJ75" s="110">
+        <v>0.00041</v>
       </c>
     </row>
     <row r="76" ht="15" customHeight="1">
@@ -55887,8 +55669,8 @@
       <c r="AI76" s="104">
         <v>0.00036</v>
       </c>
-      <c r="AJ76" t="s" s="36">
-        <v>604</v>
+      <c r="AJ76" s="110">
+        <v>0.000431</v>
       </c>
     </row>
     <row r="77" ht="15" customHeight="1">
@@ -55997,8 +55779,8 @@
       <c r="AI77" s="104">
         <v>0.00039</v>
       </c>
-      <c r="AJ77" t="s" s="36">
-        <v>605</v>
+      <c r="AJ77" s="110">
+        <v>0.00058</v>
       </c>
     </row>
     <row r="78" ht="15" customHeight="1">
@@ -56107,8 +55889,8 @@
       <c r="AI78" s="104">
         <v>0.000297</v>
       </c>
-      <c r="AJ78" t="s" s="36">
-        <v>606</v>
+      <c r="AJ78" s="110">
+        <v>0.000437</v>
       </c>
     </row>
     <row r="79" ht="15" customHeight="1">
@@ -56217,8 +55999,8 @@
       <c r="AI79" s="104">
         <v>0.000251</v>
       </c>
-      <c r="AJ79" t="s" s="36">
-        <v>607</v>
+      <c r="AJ79" s="110">
+        <v>0.000185</v>
       </c>
     </row>
   </sheetData>
@@ -56238,43 +56020,43 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.85156" style="110" customWidth="1"/>
-    <col min="2" max="2" width="9.85156" style="110" customWidth="1"/>
-    <col min="3" max="3" width="9.85156" style="110" customWidth="1"/>
-    <col min="4" max="4" width="9.85156" style="110" customWidth="1"/>
-    <col min="5" max="5" width="9.85156" style="110" customWidth="1"/>
-    <col min="6" max="6" width="9.85156" style="110" customWidth="1"/>
-    <col min="7" max="7" width="9.85156" style="110" customWidth="1"/>
-    <col min="8" max="8" width="9.85156" style="110" customWidth="1"/>
-    <col min="9" max="9" width="9.85156" style="110" customWidth="1"/>
-    <col min="10" max="10" width="9.85156" style="110" customWidth="1"/>
-    <col min="11" max="11" width="9.85156" style="110" customWidth="1"/>
-    <col min="12" max="12" width="9.85156" style="110" customWidth="1"/>
-    <col min="13" max="13" width="9.85156" style="110" customWidth="1"/>
-    <col min="14" max="14" width="9.85156" style="110" customWidth="1"/>
-    <col min="15" max="15" width="9.85156" style="110" customWidth="1"/>
-    <col min="16" max="16" width="9.85156" style="110" customWidth="1"/>
-    <col min="17" max="17" width="9.85156" style="110" customWidth="1"/>
-    <col min="18" max="18" width="9.85156" style="110" customWidth="1"/>
-    <col min="19" max="19" width="9.85156" style="110" customWidth="1"/>
-    <col min="20" max="20" width="9.85156" style="110" customWidth="1"/>
-    <col min="21" max="21" width="9.85156" style="110" customWidth="1"/>
-    <col min="22" max="22" width="9.85156" style="110" customWidth="1"/>
-    <col min="23" max="23" width="9.85156" style="110" customWidth="1"/>
-    <col min="24" max="24" width="9.85156" style="110" customWidth="1"/>
-    <col min="25" max="25" width="9.85156" style="110" customWidth="1"/>
-    <col min="26" max="26" width="9.17188" style="110" customWidth="1"/>
-    <col min="27" max="27" width="9.85156" style="110" customWidth="1"/>
-    <col min="28" max="28" width="9.85156" style="110" customWidth="1"/>
-    <col min="29" max="29" width="9.85156" style="110" customWidth="1"/>
-    <col min="30" max="30" width="9.85156" style="110" customWidth="1"/>
-    <col min="31" max="31" width="9.85156" style="110" customWidth="1"/>
-    <col min="32" max="32" width="9.85156" style="110" customWidth="1"/>
-    <col min="33" max="33" width="9.85156" style="110" customWidth="1"/>
-    <col min="34" max="34" width="9.85156" style="110" customWidth="1"/>
-    <col min="35" max="35" width="10.6719" style="110" customWidth="1"/>
-    <col min="36" max="36" width="11.8516" style="110" customWidth="1"/>
-    <col min="37" max="256" width="11.5" style="110" customWidth="1"/>
+    <col min="1" max="1" width="9.85156" style="111" customWidth="1"/>
+    <col min="2" max="2" width="9.85156" style="111" customWidth="1"/>
+    <col min="3" max="3" width="9.85156" style="111" customWidth="1"/>
+    <col min="4" max="4" width="9.85156" style="111" customWidth="1"/>
+    <col min="5" max="5" width="9.85156" style="111" customWidth="1"/>
+    <col min="6" max="6" width="9.85156" style="111" customWidth="1"/>
+    <col min="7" max="7" width="9.85156" style="111" customWidth="1"/>
+    <col min="8" max="8" width="9.85156" style="111" customWidth="1"/>
+    <col min="9" max="9" width="9.85156" style="111" customWidth="1"/>
+    <col min="10" max="10" width="9.85156" style="111" customWidth="1"/>
+    <col min="11" max="11" width="9.85156" style="111" customWidth="1"/>
+    <col min="12" max="12" width="9.85156" style="111" customWidth="1"/>
+    <col min="13" max="13" width="9.85156" style="111" customWidth="1"/>
+    <col min="14" max="14" width="9.85156" style="111" customWidth="1"/>
+    <col min="15" max="15" width="9.85156" style="111" customWidth="1"/>
+    <col min="16" max="16" width="9.85156" style="111" customWidth="1"/>
+    <col min="17" max="17" width="9.85156" style="111" customWidth="1"/>
+    <col min="18" max="18" width="9.85156" style="111" customWidth="1"/>
+    <col min="19" max="19" width="9.85156" style="111" customWidth="1"/>
+    <col min="20" max="20" width="9.85156" style="111" customWidth="1"/>
+    <col min="21" max="21" width="9.85156" style="111" customWidth="1"/>
+    <col min="22" max="22" width="9.85156" style="111" customWidth="1"/>
+    <col min="23" max="23" width="9.85156" style="111" customWidth="1"/>
+    <col min="24" max="24" width="9.85156" style="111" customWidth="1"/>
+    <col min="25" max="25" width="9.85156" style="111" customWidth="1"/>
+    <col min="26" max="26" width="9.17188" style="111" customWidth="1"/>
+    <col min="27" max="27" width="9.85156" style="111" customWidth="1"/>
+    <col min="28" max="28" width="9.85156" style="111" customWidth="1"/>
+    <col min="29" max="29" width="9.85156" style="111" customWidth="1"/>
+    <col min="30" max="30" width="9.85156" style="111" customWidth="1"/>
+    <col min="31" max="31" width="9.85156" style="111" customWidth="1"/>
+    <col min="32" max="32" width="9.85156" style="111" customWidth="1"/>
+    <col min="33" max="33" width="9.85156" style="111" customWidth="1"/>
+    <col min="34" max="34" width="9.85156" style="111" customWidth="1"/>
+    <col min="35" max="35" width="10.6719" style="111" customWidth="1"/>
+    <col min="36" max="36" width="11.8516" style="111" customWidth="1"/>
+    <col min="37" max="256" width="11.5" style="111" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -56384,7 +56166,7 @@
         <v>0.005555</v>
       </c>
       <c r="AJ1" t="s" s="36">
-        <v>608</v>
+        <v>532</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1">
@@ -56494,7 +56276,7 @@
         <v>0.004917</v>
       </c>
       <c r="AJ2" t="s" s="36">
-        <v>609</v>
+        <v>533</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
@@ -56604,7 +56386,7 @@
         <v>0.006854</v>
       </c>
       <c r="AJ3" t="s" s="36">
-        <v>610</v>
+        <v>534</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
@@ -56714,7 +56496,7 @@
         <v>0.005431</v>
       </c>
       <c r="AJ4" t="s" s="36">
-        <v>611</v>
+        <v>535</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
@@ -56824,7 +56606,7 @@
         <v>0.005639</v>
       </c>
       <c r="AJ5" t="s" s="36">
-        <v>612</v>
+        <v>536</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
@@ -56934,7 +56716,7 @@
         <v>0.005365</v>
       </c>
       <c r="AJ6" t="s" s="36">
-        <v>613</v>
+        <v>537</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
@@ -57044,7 +56826,7 @@
         <v>0.006214</v>
       </c>
       <c r="AJ7" t="s" s="36">
-        <v>614</v>
+        <v>538</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">
@@ -57154,7 +56936,7 @@
         <v>0.004961</v>
       </c>
       <c r="AJ8" t="s" s="36">
-        <v>615</v>
+        <v>539</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1">
@@ -57264,7 +57046,7 @@
         <v>0.005573</v>
       </c>
       <c r="AJ9" t="s" s="36">
-        <v>616</v>
+        <v>540</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
@@ -57374,7 +57156,7 @@
         <v>0.004782</v>
       </c>
       <c r="AJ10" t="s" s="36">
-        <v>617</v>
+        <v>541</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1">
@@ -57484,7 +57266,7 @@
         <v>0.004946</v>
       </c>
       <c r="AJ11" t="s" s="36">
-        <v>618</v>
+        <v>542</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1">
@@ -57594,7 +57376,7 @@
         <v>0.004504</v>
       </c>
       <c r="AJ12" t="s" s="36">
-        <v>619</v>
+        <v>543</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1">
@@ -57704,7 +57486,7 @@
         <v>0.004435</v>
       </c>
       <c r="AJ13" t="s" s="36">
-        <v>620</v>
+        <v>544</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1">
@@ -57814,7 +57596,7 @@
         <v>0.004382</v>
       </c>
       <c r="AJ14" t="s" s="36">
-        <v>539</v>
+        <v>545</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1">
@@ -57924,7 +57706,7 @@
         <v>0.004496</v>
       </c>
       <c r="AJ15" t="s" s="36">
-        <v>621</v>
+        <v>546</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1">
@@ -58034,7 +57816,7 @@
         <v>0.004045</v>
       </c>
       <c r="AJ16" t="s" s="36">
-        <v>622</v>
+        <v>547</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1">
@@ -58144,7 +57926,7 @@
         <v>0.003921</v>
       </c>
       <c r="AJ17" t="s" s="36">
-        <v>623</v>
+        <v>548</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1">
@@ -58254,7 +58036,7 @@
         <v>0.003827</v>
       </c>
       <c r="AJ18" t="s" s="36">
-        <v>624</v>
+        <v>549</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1">
@@ -58364,7 +58146,7 @@
         <v>0.003726</v>
       </c>
       <c r="AJ19" t="s" s="36">
-        <v>625</v>
+        <v>550</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1">
@@ -58474,7 +58256,7 @@
         <v>0.003647</v>
       </c>
       <c r="AJ20" t="s" s="36">
-        <v>626</v>
+        <v>551</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1">
@@ -58584,7 +58366,7 @@
         <v>0.00355</v>
       </c>
       <c r="AJ21" t="s" s="36">
-        <v>627</v>
+        <v>552</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1">
@@ -58694,7 +58476,7 @@
         <v>0.003476</v>
       </c>
       <c r="AJ22" t="s" s="36">
-        <v>628</v>
+        <v>553</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1">
@@ -58804,7 +58586,7 @@
         <v>0.003398</v>
       </c>
       <c r="AJ23" t="s" s="36">
-        <v>629</v>
+        <v>554</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1">
@@ -58914,7 +58696,7 @@
         <v>0.003433</v>
       </c>
       <c r="AJ24" t="s" s="36">
-        <v>630</v>
+        <v>555</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1">
@@ -59024,7 +58806,7 @@
         <v>0.003255</v>
       </c>
       <c r="AJ25" t="s" s="36">
-        <v>631</v>
+        <v>556</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1">
@@ -59134,7 +58916,7 @@
         <v>0.00299</v>
       </c>
       <c r="AJ26" t="s" s="36">
-        <v>632</v>
+        <v>557</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1">
@@ -59244,7 +59026,7 @@
         <v>0.003251</v>
       </c>
       <c r="AJ27" t="s" s="36">
-        <v>633</v>
+        <v>558</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1">
@@ -59354,7 +59136,7 @@
         <v>0.003023</v>
       </c>
       <c r="AJ28" t="s" s="36">
-        <v>634</v>
+        <v>559</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1">
@@ -59464,7 +59246,7 @@
         <v>0.002938</v>
       </c>
       <c r="AJ29" t="s" s="36">
-        <v>635</v>
+        <v>560</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1">
@@ -59574,7 +59356,7 @@
         <v>0.002866</v>
       </c>
       <c r="AJ30" t="s" s="36">
-        <v>636</v>
+        <v>561</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1">
@@ -59684,7 +59466,7 @@
         <v>0.002863</v>
       </c>
       <c r="AJ31" t="s" s="36">
-        <v>637</v>
+        <v>562</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1">
@@ -59794,7 +59576,7 @@
         <v>0.002679</v>
       </c>
       <c r="AJ32" t="s" s="36">
-        <v>638</v>
+        <v>563</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1">
@@ -59904,7 +59686,7 @@
         <v>0.002699</v>
       </c>
       <c r="AJ33" t="s" s="36">
-        <v>639</v>
+        <v>564</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1">
@@ -60014,7 +59796,7 @@
         <v>0.002535</v>
       </c>
       <c r="AJ34" t="s" s="36">
-        <v>640</v>
+        <v>565</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1">
@@ -60124,7 +59906,7 @@
         <v>0.00249</v>
       </c>
       <c r="AJ35" t="s" s="36">
-        <v>641</v>
+        <v>566</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1">
@@ -60234,7 +60016,7 @@
         <v>0.002475</v>
       </c>
       <c r="AJ36" t="s" s="36">
-        <v>642</v>
+        <v>567</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1">
@@ -60344,7 +60126,7 @@
         <v>0.002315</v>
       </c>
       <c r="AJ37" t="s" s="36">
-        <v>643</v>
+        <v>568</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1">
@@ -60454,7 +60236,7 @@
         <v>0.00238</v>
       </c>
       <c r="AJ38" t="s" s="36">
-        <v>644</v>
+        <v>569</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1">
@@ -60564,7 +60346,7 @@
         <v>0.002233</v>
       </c>
       <c r="AJ39" t="s" s="36">
-        <v>645</v>
+        <v>570</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1">
@@ -60674,7 +60456,7 @@
         <v>0.002062</v>
       </c>
       <c r="AJ40" t="s" s="36">
-        <v>646</v>
+        <v>571</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1">
@@ -60784,7 +60566,7 @@
         <v>0.002114</v>
       </c>
       <c r="AJ41" t="s" s="36">
-        <v>647</v>
+        <v>572</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1">
@@ -60894,7 +60676,7 @@
         <v>0.001922</v>
       </c>
       <c r="AJ42" t="s" s="36">
-        <v>648</v>
+        <v>573</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1">
@@ -61004,7 +60786,7 @@
         <v>0.001798</v>
       </c>
       <c r="AJ43" t="s" s="36">
-        <v>649</v>
+        <v>574</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1">
@@ -61114,7 +60896,7 @@
         <v>0.001872</v>
       </c>
       <c r="AJ44" t="s" s="36">
-        <v>650</v>
+        <v>575</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1">
@@ -61224,7 +61006,7 @@
         <v>0.001698</v>
       </c>
       <c r="AJ45" t="s" s="36">
-        <v>651</v>
+        <v>576</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1">
@@ -61334,7 +61116,7 @@
         <v>0.001676</v>
       </c>
       <c r="AJ46" t="s" s="36">
-        <v>543</v>
+        <v>577</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1">
@@ -61444,7 +61226,7 @@
         <v>0.001629</v>
       </c>
       <c r="AJ47" t="s" s="36">
-        <v>652</v>
+        <v>578</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1">
@@ -61554,7 +61336,7 @@
         <v>0.001561</v>
       </c>
       <c r="AJ48" t="s" s="36">
-        <v>653</v>
+        <v>579</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1">
@@ -61664,7 +61446,7 @@
         <v>0.001579</v>
       </c>
       <c r="AJ49" t="s" s="36">
-        <v>654</v>
+        <v>580</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1">
@@ -61774,7 +61556,7 @@
         <v>0.001467</v>
       </c>
       <c r="AJ50" t="s" s="36">
-        <v>655</v>
+        <v>581</v>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1">
@@ -61884,7 +61666,7 @@
         <v>0.001482</v>
       </c>
       <c r="AJ51" t="s" s="36">
-        <v>656</v>
+        <v>582</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1">
@@ -61994,7 +61776,7 @@
         <v>0.001437</v>
       </c>
       <c r="AJ52" t="s" s="36">
-        <v>657</v>
+        <v>583</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1">
@@ -62104,7 +61886,7 @@
         <v>0.001443</v>
       </c>
       <c r="AJ53" t="s" s="36">
-        <v>658</v>
+        <v>584</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1">
@@ -62214,7 +61996,7 @@
         <v>0.001389</v>
       </c>
       <c r="AJ54" t="s" s="36">
-        <v>659</v>
+        <v>585</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1">
@@ -62324,7 +62106,7 @@
         <v>0.001372</v>
       </c>
       <c r="AJ55" t="s" s="36">
-        <v>660</v>
+        <v>586</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1">
@@ -62434,7 +62216,7 @@
         <v>0.001402</v>
       </c>
       <c r="AJ56" t="s" s="36">
-        <v>661</v>
+        <v>587</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1">
@@ -62544,7 +62326,7 @@
         <v>0.00139</v>
       </c>
       <c r="AJ57" t="s" s="36">
-        <v>662</v>
+        <v>588</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1">
@@ -62654,7 +62436,7 @@
         <v>0.00141</v>
       </c>
       <c r="AJ58" t="s" s="36">
-        <v>663</v>
+        <v>589</v>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1">
@@ -62764,7 +62546,7 @@
         <v>0.001326</v>
       </c>
       <c r="AJ59" t="s" s="36">
-        <v>664</v>
+        <v>590</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1">
@@ -62874,7 +62656,7 @@
         <v>0.001288</v>
       </c>
       <c r="AJ60" t="s" s="36">
-        <v>665</v>
+        <v>591</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1">
@@ -62984,7 +62766,7 @@
         <v>0.001387</v>
       </c>
       <c r="AJ61" t="s" s="36">
-        <v>666</v>
+        <v>592</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1">
@@ -63094,7 +62876,7 @@
         <v>0.001273</v>
       </c>
       <c r="AJ62" t="s" s="36">
-        <v>667</v>
+        <v>593</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1">
@@ -63204,7 +62986,7 @@
         <v>0.001302</v>
       </c>
       <c r="AJ63" t="s" s="36">
-        <v>668</v>
+        <v>594</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1">
@@ -63314,7 +63096,7 @@
         <v>0.001325</v>
       </c>
       <c r="AJ64" t="s" s="36">
-        <v>669</v>
+        <v>595</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1">
@@ -63424,7 +63206,7 @@
         <v>0.001109</v>
       </c>
       <c r="AJ65" t="s" s="36">
-        <v>670</v>
+        <v>596</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1">
@@ -63534,7 +63316,7 @@
         <v>0.001153</v>
       </c>
       <c r="AJ66" t="s" s="36">
-        <v>671</v>
+        <v>597</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1">
@@ -63644,7 +63426,7 @@
         <v>0.001041</v>
       </c>
       <c r="AJ67" t="s" s="36">
-        <v>672</v>
+        <v>598</v>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1">
@@ -63754,7 +63536,7 @@
         <v>0.000876</v>
       </c>
       <c r="AJ68" t="s" s="36">
-        <v>673</v>
+        <v>599</v>
       </c>
     </row>
     <row r="69" ht="15" customHeight="1">
@@ -63864,7 +63646,7 @@
         <v>0.001064</v>
       </c>
       <c r="AJ69" t="s" s="36">
-        <v>674</v>
+        <v>600</v>
       </c>
     </row>
     <row r="70" ht="15" customHeight="1">
@@ -63974,7 +63756,7 @@
         <v>0.000699</v>
       </c>
       <c r="AJ70" t="s" s="36">
-        <v>675</v>
+        <v>601</v>
       </c>
     </row>
     <row r="71" ht="15" customHeight="1">
@@ -64084,7 +63866,7 @@
         <v>0.000636</v>
       </c>
       <c r="AJ71" t="s" s="36">
-        <v>676</v>
+        <v>602</v>
       </c>
     </row>
     <row r="72" ht="15" customHeight="1">
@@ -64194,7 +63976,7 @@
         <v>0.0007739999999999999</v>
       </c>
       <c r="AJ72" t="s" s="36">
-        <v>677</v>
+        <v>603</v>
       </c>
     </row>
     <row r="73" ht="15" customHeight="1">
@@ -64304,7 +64086,7 @@
         <v>0.000464</v>
       </c>
       <c r="AJ73" t="s" s="36">
-        <v>678</v>
+        <v>604</v>
       </c>
     </row>
     <row r="74" ht="15" customHeight="1">
@@ -64414,7 +64196,7 @@
         <v>0.000477</v>
       </c>
       <c r="AJ74" t="s" s="36">
-        <v>679</v>
+        <v>605</v>
       </c>
     </row>
     <row r="75" ht="15" customHeight="1">
@@ -64524,7 +64306,7 @@
         <v>0.000555</v>
       </c>
       <c r="AJ75" t="s" s="36">
-        <v>680</v>
+        <v>606</v>
       </c>
     </row>
     <row r="76" ht="15" customHeight="1">
@@ -64634,7 +64416,7 @@
         <v>0.000293</v>
       </c>
       <c r="AJ76" t="s" s="36">
-        <v>681</v>
+        <v>607</v>
       </c>
     </row>
     <row r="77" ht="15" customHeight="1">
@@ -64744,7 +64526,7 @@
         <v>0.0004929999999999999</v>
       </c>
       <c r="AJ77" t="s" s="36">
-        <v>682</v>
+        <v>608</v>
       </c>
     </row>
     <row r="78" ht="15" customHeight="1">
@@ -64854,7 +64636,7 @@
         <v>0.000514</v>
       </c>
       <c r="AJ78" t="s" s="36">
-        <v>683</v>
+        <v>609</v>
       </c>
     </row>
     <row r="79" ht="15" customHeight="1">
@@ -64964,7 +64746,7 @@
         <v>-0.000778</v>
       </c>
       <c r="AJ79" t="s" s="36">
-        <v>684</v>
+        <v>610</v>
       </c>
     </row>
   </sheetData>

</xml_diff>